<commit_message>
Curation WP5189 WP5172 WP5176
- Syntax is valid
</commit_message>
<xml_diff>
--- a/ValidateData/WP5172.xlsx
+++ b/ValidateData/WP5172.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
   <si>
     <t xml:space="preserve">EnzymePW</t>
   </si>
@@ -257,12 +257,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,7 +290,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Q1"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -372,22 +368,22 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="1" t="n">
         <v>30404</v>
       </c>
       <c r="G2" s="0" t="n">
@@ -396,48 +392,48 @@
       <c r="I2" s="0" t="n">
         <v>0.074</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="2" t="n">
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="M2" s="2" t="n">
+      <c r="M2" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="N2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>18498772</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="1" t="n">
         <v>11149</v>
       </c>
       <c r="G3" s="0" t="n">
@@ -446,48 +442,48 @@
       <c r="I3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="1" t="n">
         <v>11149</v>
       </c>
       <c r="G4" s="0" t="n">
@@ -496,49 +492,49 @@
       <c r="I4" s="0" t="n">
         <v>0.004</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="J4" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="L4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="M4" s="2" t="n">
+      <c r="M4" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="P4" s="1" t="n">
         <v>22961397</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>22</v>
+      <c r="F5" s="2" t="n">
+        <v>30404</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>29034</v>
@@ -546,48 +542,48 @@
       <c r="I5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="2" t="s">
+      <c r="J5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="1" t="n">
         <v>11149</v>
       </c>
       <c r="G6" s="0" t="n">
@@ -596,48 +592,48 @@
       <c r="I6" s="0" t="n">
         <v>0.0006</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="2" t="n">
+      <c r="J6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="M6" s="2" t="n">
+      <c r="M6" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" s="2" t="s">
+      <c r="N6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="P6" s="1" t="n">
         <v>775938</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="1" t="n">
         <v>11149</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -646,48 +642,48 @@
       <c r="I7" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="2" t="n">
+      <c r="J7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="M7" s="2" t="n">
+      <c r="M7" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="2" t="s">
+      <c r="N7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="P7" s="1" t="n">
         <v>775938</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q7" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="1" t="n">
         <v>16374</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -696,28 +692,28 @@
       <c r="I8" s="0" t="n">
         <v>0.017</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="2" t="n">
+      <c r="J8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="1" t="n">
         <v>7.5</v>
       </c>
-      <c r="M8" s="2" t="n">
+      <c r="M8" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="2" t="s">
+      <c r="N8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="P8" s="0" t="n">
         <v>30927326</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="1" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>